<commit_message>
Added patch antennae on separate version of Z-
</commit_message>
<xml_diff>
--- a/manufacturing/BOMs/All ICs.xlsx
+++ b/manufacturing/BOMs/All ICs.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24701"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nitro5\Documents\EAGLE\projects\CubeSat-ADCS-Hardware\manufacturing\BOMs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jasper Grant\Documents\EAGLE\projects\CubeSat-ADCS-Hardware\manufacturing\BOMs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71FA82C4-5734-4FB5-B61D-5713822ECC8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97908756-EC65-492F-B292-20440A06BBBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="117">
   <si>
     <t>Texas Instruments</t>
   </si>
@@ -361,6 +361,21 @@
   </si>
   <si>
     <t>Not in stock, alternative available</t>
+  </si>
+  <si>
+    <t>No soldering</t>
+  </si>
+  <si>
+    <t>Soldering</t>
+  </si>
+  <si>
+    <t>Desoldering</t>
+  </si>
+  <si>
+    <t>Solderinng</t>
+  </si>
+  <si>
+    <t>No Soldering</t>
   </si>
 </sst>
 </file>
@@ -768,8 +783,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AN45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="M4" sqref="M4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N19" sqref="N19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -778,7 +793,7 @@
     <col min="4" max="4" width="14.109375" customWidth="1"/>
     <col min="5" max="5" width="12.44140625" customWidth="1"/>
     <col min="6" max="6" width="12.109375" customWidth="1"/>
-    <col min="8" max="8" width="57.88671875" customWidth="1"/>
+    <col min="8" max="8" width="17.21875" customWidth="1"/>
     <col min="10" max="10" width="20.109375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -882,6 +897,9 @@
       <c r="M2" s="11" t="s">
         <v>104</v>
       </c>
+      <c r="N2" s="11" t="s">
+        <v>115</v>
+      </c>
     </row>
     <row r="3" spans="1:40" s="11" customFormat="1" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3" s="11">
@@ -917,6 +935,9 @@
       <c r="M3" s="11" t="s">
         <v>105</v>
       </c>
+      <c r="N3" s="11" t="s">
+        <v>114</v>
+      </c>
     </row>
     <row r="4" spans="1:40" s="3" customFormat="1" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B4" s="3">
@@ -952,6 +973,9 @@
       <c r="M4" s="3" t="s">
         <v>111</v>
       </c>
+      <c r="N4" s="3" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="5" spans="1:40" s="11" customFormat="1" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B5" s="11">
@@ -987,6 +1011,9 @@
       <c r="M5" s="11" t="s">
         <v>106</v>
       </c>
+      <c r="N5" s="11" t="s">
+        <v>112</v>
+      </c>
     </row>
     <row r="6" spans="1:40" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B6" s="3">
@@ -1022,6 +1049,9 @@
       <c r="M6" s="3" t="s">
         <v>107</v>
       </c>
+      <c r="N6" s="3" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="7" spans="1:40" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B7" s="11">
@@ -1057,6 +1087,9 @@
       <c r="M7" s="11" t="s">
         <v>78</v>
       </c>
+      <c r="N7" s="11" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="8" spans="1:40" s="15" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B8" s="15">
@@ -1092,7 +1125,9 @@
       <c r="M8" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="N8" s="16"/>
+      <c r="N8" s="16" t="s">
+        <v>114</v>
+      </c>
     </row>
     <row r="9" spans="1:40" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B9" s="15">
@@ -1128,7 +1163,9 @@
       <c r="M9" s="15" t="s">
         <v>110</v>
       </c>
-      <c r="N9" s="16"/>
+      <c r="N9" s="16" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="10" spans="1:40" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B10" s="15">
@@ -1164,7 +1201,9 @@
       <c r="M10" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="N10" s="16"/>
+      <c r="N10" s="16" t="s">
+        <v>116</v>
+      </c>
     </row>
     <row r="11" spans="1:40" s="15" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B11" s="15">
@@ -1200,7 +1239,9 @@
       <c r="M11" s="15" t="s">
         <v>41</v>
       </c>
-      <c r="N11" s="16"/>
+      <c r="N11" s="16" t="s">
+        <v>112</v>
+      </c>
     </row>
     <row r="12" spans="1:40" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B12" s="15">
@@ -1236,7 +1277,9 @@
       <c r="M12" s="15" t="s">
         <v>48</v>
       </c>
-      <c r="N12" s="16"/>
+      <c r="N12" s="16" t="s">
+        <v>114</v>
+      </c>
     </row>
     <row r="13" spans="1:40" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B13" s="1">
@@ -1272,7 +1315,9 @@
       <c r="M13" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="N13" s="2"/>
+      <c r="N13" s="2" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="14" spans="1:40" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B14" s="1">
@@ -1308,7 +1353,9 @@
       <c r="M14" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="N14" s="2"/>
+      <c r="N14" s="2" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="40" spans="1:1" ht="13.8" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="45" spans="1:1" x14ac:dyDescent="0.3">

</xml_diff>